<commit_message>
Tabelle zur Dokumentation der Prüfstandsversuche vorbereitet
</commit_message>
<xml_diff>
--- a/AI_MOLE/Test_Bench/Torsion_Oszillator/Experiment_log.xlsx
+++ b/AI_MOLE/Test_Bench/Torsion_Oszillator/Experiment_log.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung_Ole\Masterarbeit_AI_MOLE\AI_MOLE\Test_Bench\Torsion_Oszillator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908B67E6-BE9B-4E5D-AB01-ABEA0162B94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Versuchsprotokoll (MOLE)" sheetId="1" r:id="rId1"/>
+    <sheet name="Referenztrajektorien" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,10 +25,122 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Dateiname</t>
+  </si>
+  <si>
+    <t>Architektur</t>
+  </si>
+  <si>
+    <t>Referenztrajektorie</t>
+  </si>
+  <si>
+    <t>Iterationen</t>
+  </si>
+  <si>
+    <t>Nichtlin. Dämpfung</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>ILC Methode</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Simulation/Trial</t>
+  </si>
+  <si>
+    <t>Run_01_uncontrolled</t>
+  </si>
+  <si>
+    <t>Stochastic</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Uncontrolled</t>
+  </si>
+  <si>
+    <t>Trajectory_01</t>
+  </si>
+  <si>
+    <t>Simulation mit veralteter Version</t>
+  </si>
+  <si>
+    <t>Run_01_serial</t>
+  </si>
+  <si>
+    <t>Serial (feedforward)</t>
+  </si>
+  <si>
+    <t>Trajectory_02</t>
+  </si>
+  <si>
+    <t>relative_2</t>
+  </si>
+  <si>
+    <t>Testlauf Simulation</t>
+  </si>
+  <si>
+    <t>GP Trainingsdaten H</t>
+  </si>
+  <si>
+    <t>In Thesis Nutzen</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>Abtastzeit Ts [s]</t>
+  </si>
+  <si>
+    <t>Länge [s]</t>
+  </si>
+  <si>
+    <t>Stetig differenzierbar</t>
+  </si>
+  <si>
+    <t>Amplidude [rad]</t>
+  </si>
+  <si>
+    <t>Generierung</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>C-2</t>
+  </si>
+  <si>
+    <t>Quinticpolytraj</t>
+  </si>
+  <si>
+    <t>Einfacher, stetiger Winkelübergang</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,13 +168,129 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +301,43 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}" name="Tabelle1" displayName="Tabelle1" ref="A1:L3" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:L3" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{57E8A950-5641-4CEF-96CF-9E419B47D19C}" name="Datum" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{91C5A9D0-5D8D-4481-8037-952760167E31}" name="Dateiname" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{6C4C4FC7-AEDA-40E0-BCB3-0FC0B06704B5}" name="Architektur" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{ECF07697-4061-4D2F-9A88-D323B40A7FA4}" name="Referenztrajektorie" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{83C385E2-DC6F-4790-85F5-90962D5D4E1D}" name="Iterationen" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{E04CDD9F-FA6F-4DD7-A3BB-7F42717DB8E8}" name="GP Trainingsdaten H" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{E6B6ED04-813F-4794-A91D-E69D682BE652}" name="Nichtlin. Dämpfung" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{04DB29C6-D7C8-4D58-BDE3-45C85F93E9B9}" name="Beta" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{D83E9EBA-F307-4D7E-A5D1-1CAD99A95A1A}" name="ILC Methode" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{483D8DDD-C993-401D-BE6B-2C6661119950}" name="Simulation/Trial" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{5621DE79-5887-4488-8E2C-981858CBF030}" name="In Thesis Nutzen" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{0A3B22CE-0BDD-4AAD-88BA-74D4E16CF1D6}" name="Kommentar"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43DA8F1D-6502-4878-8009-693EAB99A35A}" name="Tabelle2" displayName="Tabelle2" ref="A1:G3" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:G3" xr:uid="{43DA8F1D-6502-4878-8009-693EAB99A35A}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{1FA48B55-6A3F-4007-B441-9696E9D798AA}" name="Dateiname" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{EDF3DA31-D44E-4CB4-A1F9-F4CABAFCB2AD}" name="Abtastzeit Ts [s]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{7853305C-6404-4C46-B7D0-C621C014B499}" name="Länge [s]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{0B5D86BE-6CB1-4700-B1B2-3D69F671D7F3}" name="Stetig differenzierbar" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{DDCC3695-80CA-4EBC-AFBC-ABD992ADADA3}" name="Amplidude [rad]" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{1AB2223B-0903-41C5-8B52-EBE451C3BCBE}" name="Generierung" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{CAC3A8CC-8538-422D-9654-D9FF00DBDA23}" name="Beschreibung" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +602,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>46020</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>46030</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9381838-4D60-4571-ADD6-94E4FB4B0EC8}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="3"/>
+    <col min="4" max="4" width="22.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3">
+        <v>24.4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update der excel tabelle
</commit_message>
<xml_diff>
--- a/AI_MOLE/Test_Bench/Torsion_Oszillator/Experiment_log.xlsx
+++ b/AI_MOLE/Test_Bench/Torsion_Oszillator/Experiment_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung_Ole\Masterarbeit_AI_MOLE\AI_MOLE\Test_Bench\Torsion_Oszillator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908B67E6-BE9B-4E5D-AB01-ABEA0162B94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A27CDA-05F4-42F1-AF35-AF16DA80CDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versuchsprotokoll (MOLE)" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Datum</t>
   </si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>Einfacher, stetiger Winkelübergang</t>
+  </si>
+  <si>
+    <t>Erster Testlauf am Prüfstand, Funktion zur Nullung des Eingangssignals vor Versuchsbeginn in Simulink erst mittendrin hinzugefügt</t>
   </si>
 </sst>
 </file>
@@ -170,7 +176,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -186,11 +191,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -214,30 +249,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -304,37 +315,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}" name="Tabelle1" displayName="Tabelle1" ref="A1:L3" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:L3" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}" name="Tabelle1" displayName="Tabelle1" ref="A1:L4" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:L4" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{57E8A950-5641-4CEF-96CF-9E419B47D19C}" name="Datum" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{91C5A9D0-5D8D-4481-8037-952760167E31}" name="Dateiname" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{6C4C4FC7-AEDA-40E0-BCB3-0FC0B06704B5}" name="Architektur" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{ECF07697-4061-4D2F-9A88-D323B40A7FA4}" name="Referenztrajektorie" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{83C385E2-DC6F-4790-85F5-90962D5D4E1D}" name="Iterationen" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{E04CDD9F-FA6F-4DD7-A3BB-7F42717DB8E8}" name="GP Trainingsdaten H" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{E6B6ED04-813F-4794-A91D-E69D682BE652}" name="Nichtlin. Dämpfung" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{04DB29C6-D7C8-4D58-BDE3-45C85F93E9B9}" name="Beta" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{D83E9EBA-F307-4D7E-A5D1-1CAD99A95A1A}" name="ILC Methode" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{483D8DDD-C993-401D-BE6B-2C6661119950}" name="Simulation/Trial" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{5621DE79-5887-4488-8E2C-981858CBF030}" name="In Thesis Nutzen" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{0A3B22CE-0BDD-4AAD-88BA-74D4E16CF1D6}" name="Kommentar"/>
+    <tableColumn id="1" xr3:uid="{57E8A950-5641-4CEF-96CF-9E419B47D19C}" name="Datum" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{91C5A9D0-5D8D-4481-8037-952760167E31}" name="Dateiname" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{6C4C4FC7-AEDA-40E0-BCB3-0FC0B06704B5}" name="Architektur" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{ECF07697-4061-4D2F-9A88-D323B40A7FA4}" name="Referenztrajektorie" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{83C385E2-DC6F-4790-85F5-90962D5D4E1D}" name="Iterationen" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{E04CDD9F-FA6F-4DD7-A3BB-7F42717DB8E8}" name="GP Trainingsdaten H" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{E6B6ED04-813F-4794-A91D-E69D682BE652}" name="Nichtlin. Dämpfung" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{04DB29C6-D7C8-4D58-BDE3-45C85F93E9B9}" name="Beta" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{D83E9EBA-F307-4D7E-A5D1-1CAD99A95A1A}" name="ILC Methode" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{483D8DDD-C993-401D-BE6B-2C6661119950}" name="Simulation/Trial" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{5621DE79-5887-4488-8E2C-981858CBF030}" name="In Thesis Nutzen" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{0A3B22CE-0BDD-4AAD-88BA-74D4E16CF1D6}" name="Kommentar" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43DA8F1D-6502-4878-8009-693EAB99A35A}" name="Tabelle2" displayName="Tabelle2" ref="A1:G3" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43DA8F1D-6502-4878-8009-693EAB99A35A}" name="Tabelle2" displayName="Tabelle2" ref="A1:G3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:G3" xr:uid="{43DA8F1D-6502-4878-8009-693EAB99A35A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1FA48B55-6A3F-4007-B441-9696E9D798AA}" name="Dateiname" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{EDF3DA31-D44E-4CB4-A1F9-F4CABAFCB2AD}" name="Abtastzeit Ts [s]" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{7853305C-6404-4C46-B7D0-C621C014B499}" name="Länge [s]" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{0B5D86BE-6CB1-4700-B1B2-3D69F671D7F3}" name="Stetig differenzierbar" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{DDCC3695-80CA-4EBC-AFBC-ABD992ADADA3}" name="Amplidude [rad]" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{1AB2223B-0903-41C5-8B52-EBE451C3BCBE}" name="Generierung" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{CAC3A8CC-8538-422D-9654-D9FF00DBDA23}" name="Beschreibung" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1FA48B55-6A3F-4007-B441-9696E9D798AA}" name="Dateiname" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{EDF3DA31-D44E-4CB4-A1F9-F4CABAFCB2AD}" name="Abtastzeit Ts [s]" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{7853305C-6404-4C46-B7D0-C621C014B499}" name="Länge [s]" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{0B5D86BE-6CB1-4700-B1B2-3D69F671D7F3}" name="Stetig differenzierbar" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{DDCC3695-80CA-4EBC-AFBC-ABD992ADADA3}" name="Amplidude [rad]" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{1AB2223B-0903-41C5-8B52-EBE451C3BCBE}" name="Generierung" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{CAC3A8CC-8538-422D-9654-D9FF00DBDA23}" name="Beschreibung" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,137 +614,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>46020</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>3</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>46030</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>3</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="6" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>46034</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -753,83 +802,83 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3"/>
-    <col min="4" max="4" width="22.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="2"/>
+    <col min="4" max="4" width="22.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.01</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>5.5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.01</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>24.4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Runs für Thesis herausgesucht
</commit_message>
<xml_diff>
--- a/AI_MOLE/Test_Bench/Torsion_Oszillator/Experiment_log.xlsx
+++ b/AI_MOLE/Test_Bench/Torsion_Oszillator/Experiment_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung_Ole\Masterarbeit_AI_MOLE\AI_MOLE\Test_Bench\Torsion_Oszillator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3804C0-6D52-404A-9409-97D17F5AC0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E482B34C-50E1-4115-9069-4348E2F305EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versuchsprotokoll (MOLE)" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="75">
   <si>
     <t>Datum</t>
   </si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>Testlauf am prüfstand zur Untersuchung des bereits simulativ betrachteten Effektes. Identischer Run wie vorher - zum Vergleich</t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
@@ -437,9 +437,19 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}" name="Tabelle1" displayName="Tabelle1" ref="A1:L28" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:L28" xr:uid="{64AE17CE-7A85-4552-B08B-1317F901654A}">
-    <filterColumn colId="2">
+    <filterColumn colId="5">
       <filters>
-        <filter val="Serial (no feedforward - sinus as initial input)"/>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Prüfstand"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="ja"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -742,27 +752,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="23" style="2" customWidth="1"/>
     <col min="7" max="7" width="22" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="30.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -800,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>46020</v>
       </c>
@@ -835,7 +845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>46030</v>
       </c>
@@ -873,7 +883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>46034</v>
       </c>
@@ -911,7 +921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>46034</v>
       </c>
@@ -949,7 +959,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>46034</v>
       </c>
@@ -987,7 +997,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>46034</v>
       </c>
@@ -1025,7 +1035,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>46035</v>
       </c>
@@ -1063,7 +1073,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>46035</v>
       </c>
@@ -1092,13 +1102,13 @@
         <v>34</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>46035</v>
       </c>
@@ -1133,7 +1143,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>46035</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>46035</v>
       </c>
@@ -1203,13 +1213,13 @@
         <v>34</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>46035</v>
       </c>
@@ -1247,7 +1257,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>46035</v>
       </c>
@@ -1282,7 +1292,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>46035</v>
       </c>
@@ -1317,7 +1327,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>46035</v>
       </c>
@@ -1352,7 +1362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>46035</v>
       </c>
@@ -1387,7 +1397,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>46035</v>
       </c>
@@ -1422,7 +1432,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>46036</v>
       </c>
@@ -1451,13 +1461,13 @@
         <v>34</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>46036</v>
       </c>
@@ -1492,7 +1502,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>46036</v>
       </c>
@@ -1524,13 +1534,13 @@
         <v>34</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>46036</v>
       </c>
@@ -1562,13 +1572,13 @@
         <v>34</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>46036</v>
       </c>
@@ -1606,7 +1616,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>46036</v>
       </c>
@@ -1644,7 +1654,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>46036</v>
       </c>
@@ -1679,7 +1689,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>46036</v>
       </c>
@@ -1714,7 +1724,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>46049</v>
       </c>
@@ -1746,13 +1756,13 @@
         <v>34</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>46049</v>
       </c>
@@ -1807,18 +1817,18 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="2"/>
-    <col min="4" max="4" width="22.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2"/>
+    <col min="4" max="4" width="22.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1841,7 +1851,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1864,7 +1874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1887,7 +1897,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>